<commit_message>
A day's work of wrangling data and producing backtracking input files to hand off to Irina.
</commit_message>
<xml_diff>
--- a/data/SlopeSeaOperations.xlsx
+++ b/data/SlopeSeaOperations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissy/JointProgram/SlopeSea/2016_data/SlopeSeaBluefinTuna/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7954E3E6-D8BF-C646-9FEE-E3FAEAC412AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1368268-BAD3-1A4F-B37A-D7D3001A62E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26880" yWindow="460" windowWidth="30840" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39680" yWindow="460" windowWidth="30840" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllSamplesToBeSorted" sheetId="1" r:id="rId1"/>
@@ -1106,6 +1106,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1162,7 +1165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1180,6 +1183,12 @@
     <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -52034,12 +52043,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BI1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="22" customWidth="1"/>
     <col min="11" max="61" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -52071,7 +52082,7 @@
       <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="17" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -52256,7 +52267,7 @@
       <c r="I2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="18">
         <v>42563.66196759259</v>
       </c>
       <c r="K2" s="6">
@@ -52425,7 +52436,7 @@
       <c r="I3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="18">
         <v>42562.376736111109</v>
       </c>
       <c r="K3" s="6">
@@ -52594,7 +52605,7 @@
       <c r="I4" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="18">
         <v>42563.925335648149</v>
       </c>
       <c r="K4" s="6">
@@ -52763,7 +52774,7 @@
       <c r="I5" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="18">
         <v>42562.665590277778</v>
       </c>
       <c r="K5" s="6">
@@ -52932,7 +52943,7 @@
       <c r="I6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="18">
         <v>42562.991168981483</v>
       </c>
       <c r="K6" s="6">
@@ -53101,7 +53112,7 @@
       <c r="I7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="18">
         <v>42563.378113425926</v>
       </c>
       <c r="K7" s="6">
@@ -53270,7 +53281,7 @@
       <c r="I8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="19">
         <v>42554.666944444441</v>
       </c>
       <c r="K8" s="1">
@@ -53431,7 +53442,7 @@
       <c r="I9" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="18">
         <v>42587.006805555553</v>
       </c>
       <c r="K9" s="6">
@@ -53600,7 +53611,7 @@
       <c r="I10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="19">
         <v>42553.354212962964</v>
       </c>
       <c r="K10" s="1">
@@ -53761,7 +53772,7 @@
       <c r="I11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="18">
         <v>42570.375740740739</v>
       </c>
       <c r="K11" s="6">
@@ -53930,7 +53941,7 @@
       <c r="I12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="19">
         <v>42576.657500000001</v>
       </c>
       <c r="K12" s="1">
@@ -54091,7 +54102,7 @@
       <c r="I13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="19">
         <v>42593.37835648148</v>
       </c>
       <c r="K13" s="1">
@@ -54252,7 +54263,7 @@
       <c r="I14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="19">
         <v>42595.927106481482</v>
       </c>
       <c r="K14" s="1">
@@ -54413,7 +54424,7 @@
       <c r="I15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="19">
         <v>42571.95380787037</v>
       </c>
       <c r="K15" s="1">
@@ -54574,7 +54585,7 @@
       <c r="I16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="19">
         <v>42596.866342592592</v>
       </c>
       <c r="K16" s="1">
@@ -54735,7 +54746,7 @@
       <c r="I17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="19">
         <v>42586.375115740739</v>
       </c>
       <c r="K17" s="1">
@@ -54896,7 +54907,7 @@
       <c r="I18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="19">
         <v>42597.927430555559</v>
       </c>
       <c r="K18" s="1">
@@ -55057,7 +55068,7 @@
       <c r="I19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="19">
         <v>42549.933576388888</v>
       </c>
       <c r="K19" s="1">
@@ -55218,7 +55229,7 @@
       <c r="I20" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="18">
         <v>42592.924456018518</v>
       </c>
       <c r="K20" s="6">
@@ -55387,7 +55398,7 @@
       <c r="I21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="19">
         <v>42575.656898148147</v>
       </c>
       <c r="K21" s="1">
@@ -55548,7 +55559,7 @@
       <c r="I22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="19">
         <v>42564.352488425924</v>
       </c>
       <c r="K22" s="1">
@@ -55709,7 +55720,7 @@
       <c r="I23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="19">
         <v>42586.653599537036</v>
       </c>
       <c r="K23" s="1">
@@ -55870,7 +55881,7 @@
       <c r="I24" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="18">
         <v>42598.356620370374</v>
       </c>
       <c r="K24" s="6">
@@ -56039,7 +56050,7 @@
       <c r="I25" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="18">
         <v>42600.364328703705</v>
       </c>
       <c r="K25" s="6">
@@ -56208,7 +56219,7 @@
       <c r="I26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="19">
         <v>42603.9371875</v>
       </c>
       <c r="K26" s="1">
@@ -56369,7 +56380,7 @@
       <c r="I27" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="18">
         <v>42598.875949074078</v>
       </c>
       <c r="K27" s="6">
@@ -56538,7 +56549,7 @@
       <c r="I28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="19">
         <v>42584.656747685185</v>
       </c>
       <c r="K28" s="1">
@@ -56699,7 +56710,7 @@
       <c r="I29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="19">
         <v>42549.418888888889</v>
       </c>
       <c r="K29" s="1">
@@ -56860,7 +56871,7 @@
       <c r="I30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="19">
         <v>42551.203634259262</v>
       </c>
       <c r="K30" s="1">
@@ -57021,7 +57032,7 @@
       <c r="I31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="19">
         <v>42581.37431712963</v>
       </c>
       <c r="K31" s="1">
@@ -57182,7 +57193,7 @@
       <c r="I32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="19">
         <v>42549.67087962963</v>
       </c>
       <c r="K32" s="1">
@@ -57343,7 +57354,7 @@
       <c r="I33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="19">
         <v>42572.657881944448</v>
       </c>
       <c r="K33" s="1">
@@ -57504,7 +57515,7 @@
       <c r="I34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="19">
         <v>42605.375844907408</v>
       </c>
       <c r="K34" s="1">
@@ -57665,7 +57676,7 @@
       <c r="I35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="19">
         <v>42559.984502314815</v>
       </c>
       <c r="K35" s="1">
@@ -57826,7 +57837,7 @@
       <c r="I36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="19">
         <v>42555.191747685189</v>
       </c>
       <c r="K36" s="1">
@@ -57987,7 +57998,7 @@
       <c r="I37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="19">
         <v>42596.356550925928</v>
       </c>
       <c r="K37" s="1">
@@ -58148,7 +58159,7 @@
       <c r="I38" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="18">
         <v>42600.963263888887</v>
       </c>
       <c r="K38" s="6">
@@ -58317,7 +58328,7 @@
       <c r="I39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="19">
         <v>42551.120833333334</v>
       </c>
       <c r="K39" s="1">
@@ -58478,7 +58489,7 @@
       <c r="I40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="19">
         <v>42554.167511574073</v>
       </c>
       <c r="K40" s="1">
@@ -58639,7 +58650,7 @@
       <c r="I41" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J41" s="7">
+      <c r="J41" s="18">
         <v>42605.658553240741</v>
       </c>
       <c r="K41" s="6">
@@ -58808,7 +58819,7 @@
       <c r="I42" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J42" s="7">
+      <c r="J42" s="18">
         <v>42605.93582175926</v>
       </c>
       <c r="K42" s="6">
@@ -58977,7 +58988,7 @@
       <c r="I43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J43" s="18">
         <v>42605.93582175926</v>
       </c>
       <c r="K43" s="6">
@@ -59146,7 +59157,7 @@
       <c r="I44" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="18">
         <v>42573.35229166667</v>
       </c>
       <c r="K44" s="6">
@@ -59315,7 +59326,7 @@
       <c r="I45" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="18">
         <v>42593.660613425927</v>
       </c>
       <c r="K45" s="6">
@@ -59484,7 +59495,7 @@
       <c r="I46" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="19">
         <v>42595.361724537041</v>
       </c>
       <c r="K46" s="1">
@@ -59648,7 +59659,7 @@
       <c r="I47" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="19">
         <v>42551.054201388892</v>
       </c>
       <c r="K47" s="1">
@@ -59809,7 +59820,7 @@
       <c r="I48" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="19">
         <v>42553.962835648148</v>
       </c>
       <c r="K48" s="1">
@@ -59970,7 +59981,7 @@
       <c r="I49" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J49" s="7">
+      <c r="J49" s="18">
         <v>42601.365925925929</v>
       </c>
       <c r="K49" s="6">
@@ -60139,7 +60150,7 @@
       <c r="I50" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="18">
         <v>42564.939293981479</v>
       </c>
       <c r="K50" s="6">
@@ -60308,7 +60319,7 @@
       <c r="I51" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="19">
         <v>42555.01295138889</v>
       </c>
       <c r="K51" s="1">
@@ -60469,7 +60480,7 @@
       <c r="I52" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="18">
         <v>42583.661469907405</v>
       </c>
       <c r="K52" s="6">
@@ -60638,7 +60649,7 @@
       <c r="I53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="19">
         <v>42572.956388888888</v>
       </c>
       <c r="K53" s="1">
@@ -60799,7 +60810,7 @@
       <c r="I54" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J54" s="7">
+      <c r="J54" s="18">
         <v>42570.909537037034</v>
       </c>
       <c r="K54" s="6">
@@ -60968,7 +60979,7 @@
       <c r="I55" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="19">
         <v>42576.372395833336</v>
       </c>
       <c r="K55" s="1">
@@ -61129,7 +61140,7 @@
       <c r="I56" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="18">
         <v>42597.6562962963</v>
       </c>
       <c r="K56" s="6">
@@ -61298,7 +61309,7 @@
       <c r="I57" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J57" s="7">
+      <c r="J57" s="18">
         <v>42601.657326388886</v>
       </c>
       <c r="K57" s="6">
@@ -61467,7 +61478,7 @@
       <c r="I58" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J58" s="7">
+      <c r="J58" s="18">
         <v>42575.419699074075</v>
       </c>
       <c r="K58" s="6">
@@ -61636,7 +61647,7 @@
       <c r="I59" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J59" s="7">
+      <c r="J59" s="18">
         <v>42601.927685185183</v>
       </c>
       <c r="K59" s="6">
@@ -61805,7 +61816,7 @@
       <c r="I60" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J60" s="7">
+      <c r="J60" s="18">
         <v>42552.161527777775</v>
       </c>
       <c r="K60" s="6">
@@ -61974,7 +61985,7 @@
       <c r="I61" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J61" s="7">
+      <c r="J61" s="18">
         <v>42598.658391203702</v>
       </c>
       <c r="K61" s="6">
@@ -62143,7 +62154,7 @@
       <c r="I62" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J62" s="7">
+      <c r="J62" s="18">
         <v>42603.345833333333</v>
       </c>
       <c r="K62" s="6">
@@ -62312,7 +62323,7 @@
       <c r="I63" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J63" s="7">
+      <c r="J63" s="18">
         <v>42581.959548611114</v>
       </c>
       <c r="K63" s="6">
@@ -62481,7 +62492,7 @@
       <c r="I64" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J64" s="19">
         <v>42576.955312500002</v>
       </c>
       <c r="K64" s="1">
@@ -62642,7 +62653,7 @@
       <c r="I65" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J65" s="7">
+      <c r="J65" s="18">
         <v>42600.658090277779</v>
       </c>
       <c r="K65" s="6">
@@ -62811,7 +62822,7 @@
       <c r="I66" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J66" s="14">
+      <c r="J66" s="20">
         <v>42584.956574074073</v>
       </c>
       <c r="K66" s="13">
@@ -62980,7 +62991,7 @@
       <c r="I67" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J67" s="14">
+      <c r="J67" s="20">
         <v>42552.246134259258</v>
       </c>
       <c r="K67" s="13">
@@ -63149,7 +63160,7 @@
       <c r="I68" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J68" s="14">
+      <c r="J68" s="20">
         <v>42578.656099537038</v>
       </c>
       <c r="K68" s="13">
@@ -63318,7 +63329,7 @@
       <c r="I69" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J69" s="14">
+      <c r="J69" s="20">
         <v>42573.657962962963</v>
       </c>
       <c r="K69" s="13">
@@ -63487,7 +63498,7 @@
       <c r="I70" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J70" s="14">
+      <c r="J70" s="20">
         <v>42593.930277777778</v>
       </c>
       <c r="K70" s="13">
@@ -63656,7 +63667,7 @@
       <c r="I71" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J71" s="10">
+      <c r="J71" s="21">
         <v>42550.968425925923</v>
       </c>
       <c r="K71" s="2">
@@ -63825,7 +63836,7 @@
       <c r="I72" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J72" s="14">
+      <c r="J72" s="20">
         <v>42597.388541666667</v>
       </c>
       <c r="K72" s="13">
@@ -63994,7 +64005,7 @@
       <c r="I73" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J73" s="14">
+      <c r="J73" s="20">
         <v>42606.388935185183</v>
       </c>
       <c r="K73" s="13">
@@ -64163,7 +64174,7 @@
       <c r="I74" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J74" s="14">
+      <c r="J74" s="20">
         <v>42581.655821759261</v>
       </c>
       <c r="K74" s="13">
@@ -64332,7 +64343,7 @@
       <c r="I75" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J75" s="14">
+      <c r="J75" s="20">
         <v>42604.97074074074</v>
       </c>
       <c r="K75" s="13">
@@ -64501,7 +64512,7 @@
       <c r="I76" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J76" s="14">
+      <c r="J76" s="20">
         <v>42602.667951388888</v>
       </c>
       <c r="K76" s="13">
@@ -64670,7 +64681,7 @@
       <c r="I77" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J77" s="14">
+      <c r="J77" s="20">
         <v>42594.385601851849</v>
       </c>
       <c r="K77" s="13">
@@ -64839,7 +64850,7 @@
       <c r="I78" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J78" s="14">
+      <c r="J78" s="20">
         <v>42604.366620370369</v>
       </c>
       <c r="K78" s="13">
@@ -65008,7 +65019,7 @@
       <c r="I79" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J79" s="14">
+      <c r="J79" s="20">
         <v>42602.938657407409</v>
       </c>
       <c r="K79" s="13">
@@ -65177,7 +65188,7 @@
       <c r="I80" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J80" s="14">
+      <c r="J80" s="20">
         <v>42579.385520833333</v>
       </c>
       <c r="K80" s="13">
@@ -65346,7 +65357,7 @@
       <c r="I81" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J81" s="14">
+      <c r="J81" s="20">
         <v>42570.66778935185</v>
       </c>
       <c r="K81" s="13">
@@ -65515,7 +65526,7 @@
       <c r="I82" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J82" s="14">
+      <c r="J82" s="20">
         <v>42571.658483796295</v>
       </c>
       <c r="K82" s="13">
@@ -65684,7 +65695,7 @@
       <c r="I83" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J83" s="14">
+      <c r="J83" s="20">
         <v>42559.167210648149</v>
       </c>
       <c r="K83" s="13">
@@ -65853,7 +65864,7 @@
       <c r="I84" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J84" s="14">
+      <c r="J84" s="20">
         <v>42583.94940972222</v>
       </c>
       <c r="K84" s="13">
@@ -66022,7 +66033,7 @@
       <c r="I85" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J85" s="14">
+      <c r="J85" s="20">
         <v>42551.666388888887</v>
       </c>
       <c r="K85" s="13">
@@ -66191,7 +66202,7 @@
       <c r="I86" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J86" s="14">
+      <c r="J86" s="20">
         <v>42564.66306712963</v>
       </c>
       <c r="K86" s="13">
@@ -66360,7 +66371,7 @@
       <c r="I87" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J87" s="14">
+      <c r="J87" s="20">
         <v>42559.107407407406</v>
       </c>
       <c r="K87" s="13">
@@ -66529,7 +66540,7 @@
       <c r="I88" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J88" s="14">
+      <c r="J88" s="20">
         <v>42596.654895833337</v>
       </c>
       <c r="K88" s="13">
@@ -66698,7 +66709,7 @@
       <c r="I89" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J89" s="14">
+      <c r="J89" s="20">
         <v>42558.986377314817</v>
       </c>
       <c r="K89" s="13">
@@ -66867,7 +66878,7 @@
       <c r="I90" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J90" s="14">
+      <c r="J90" s="20">
         <v>42554.237997685188</v>
       </c>
       <c r="K90" s="13">
@@ -67036,7 +67047,7 @@
       <c r="I91" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J91" s="14">
+      <c r="J91" s="20">
         <v>42582.948229166665</v>
       </c>
       <c r="K91" s="13">
@@ -67203,7 +67214,7 @@
       <c r="I92" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J92" s="14">
+      <c r="J92" s="20">
         <v>42603.659583333334</v>
       </c>
       <c r="K92" s="13">
@@ -67372,7 +67383,7 @@
       <c r="I93" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J93" s="14">
+      <c r="J93" s="20">
         <v>42606.65792824074</v>
       </c>
       <c r="K93" s="13">
@@ -67539,7 +67550,7 @@
       <c r="I94" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J94" s="14">
+      <c r="J94" s="20">
         <v>42555.664953703701</v>
       </c>
       <c r="K94" s="13">
@@ -67708,7 +67719,7 @@
       <c r="I95" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J95" s="14">
+      <c r="J95" s="20">
         <v>42559.059814814813</v>
       </c>
       <c r="K95" s="13">
@@ -67877,7 +67888,7 @@
       <c r="I96" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J96" s="14">
+      <c r="J96" s="20">
         <v>42556.160902777781</v>
       </c>
       <c r="K96" s="13">
@@ -68046,7 +68057,7 @@
       <c r="I97" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J97" s="14">
+      <c r="J97" s="20">
         <v>42559.66065972222</v>
       </c>
       <c r="K97" s="13">
@@ -68215,7 +68226,7 @@
       <c r="I98" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J98" s="14">
+      <c r="J98" s="20">
         <v>42582.656550925924</v>
       </c>
       <c r="K98" s="13">
@@ -68384,7 +68395,7 @@
       <c r="I99" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J99" s="14">
+      <c r="J99" s="20">
         <v>42579.659247685187</v>
       </c>
       <c r="K99" s="13">
@@ -68553,7 +68564,7 @@
       <c r="I100" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J100" s="14">
+      <c r="J100" s="20">
         <v>42604.659502314818</v>
       </c>
       <c r="K100" s="13">
@@ -68722,7 +68733,7 @@
       <c r="I101" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J101" s="14">
+      <c r="J101" s="20">
         <v>42595.658518518518</v>
       </c>
       <c r="K101" s="13">
@@ -68891,7 +68902,7 @@
       <c r="I102" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J102" s="14">
+      <c r="J102" s="20">
         <v>42580.336736111109</v>
       </c>
       <c r="K102" s="13">
@@ -69060,7 +69071,7 @@
       <c r="I103" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J103" s="14">
+      <c r="J103" s="20">
         <v>42558.660162037035</v>
       </c>
       <c r="K103" s="13">
@@ -69229,7 +69240,7 @@
       <c r="I104" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J104" s="7">
+      <c r="J104" s="18">
         <v>42556.084629629629</v>
       </c>
       <c r="K104" s="6">
@@ -69398,7 +69409,7 @@
       <c r="I105" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J105" s="7">
+      <c r="J105" s="18">
         <v>42580.657604166663</v>
       </c>
       <c r="K105" s="6">
@@ -69567,7 +69578,7 @@
       <c r="I106" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J106" s="7">
+      <c r="J106" s="18">
         <v>42573.961921296293</v>
       </c>
       <c r="K106" s="6">
@@ -69736,7 +69747,7 @@
       <c r="I107" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J107" s="7">
+      <c r="J107" s="18">
         <v>42552.016250000001</v>
       </c>
       <c r="K107" s="6">
@@ -69905,7 +69916,7 @@
       <c r="I108" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J108" s="7">
+      <c r="J108" s="18">
         <v>42552.100914351853</v>
       </c>
       <c r="K108" s="6">
@@ -70074,7 +70085,7 @@
       <c r="I109" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J109" s="7">
+      <c r="J109" s="18">
         <v>42558.107974537037</v>
       </c>
       <c r="K109" s="6">
@@ -70243,7 +70254,7 @@
       <c r="I110" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J110" s="7">
+      <c r="J110" s="18">
         <v>42552.965173611112</v>
       </c>
       <c r="K110" s="6">
@@ -70412,7 +70423,7 @@
       <c r="I111" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J111" s="7">
+      <c r="J111" s="18">
         <v>42552.662905092591</v>
       </c>
       <c r="K111" s="6">
@@ -70581,7 +70592,7 @@
       <c r="I112" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J112" s="7">
+      <c r="J112" s="18">
         <v>42555.957939814813</v>
       </c>
       <c r="K112" s="6">
@@ -70750,7 +70761,7 @@
       <c r="I113" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J113" s="7">
+      <c r="J113" s="18">
         <v>42557.956736111111</v>
       </c>
       <c r="K113" s="6">
@@ -70919,7 +70930,7 @@
       <c r="I114" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J114" s="7">
+      <c r="J114" s="18">
         <v>42557.665925925925</v>
       </c>
       <c r="K114" s="6">
@@ -71088,7 +71099,7 @@
       <c r="I115" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J115" s="7">
+      <c r="J115" s="18">
         <v>42558.028900462959</v>
       </c>
       <c r="K115" s="6">

</xml_diff>